<commit_message>
added: logging modified: handling xlsx file modified: Product class properties, from int&float to String same changes...
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\10 Скобяные изделия\Весы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ScalesPrep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,76 +27,76 @@
     <t>Штрихкод</t>
   </si>
   <si>
+    <t>Цена ₽</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 5 ММ</t>
+  </si>
+  <si>
+    <t>383,00</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 6 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 8 ММ</t>
+  </si>
+  <si>
+    <t>366,00</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 10 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 12 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 5 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 6 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 8 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 10 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 12 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 16 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 20 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 16 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 20 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.DIN 125A 14 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 14 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 18 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 22 ММ</t>
+  </si>
+  <si>
+    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 24 ММ</t>
+  </si>
+  <si>
+    <t>Номер лотка</t>
+  </si>
+  <si>
     <t>Наименование</t>
-  </si>
-  <si>
-    <t>Цена ₽</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 5 ММ</t>
-  </si>
-  <si>
-    <t>383,00</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 6 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 8 ММ</t>
-  </si>
-  <si>
-    <t>366,00</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 10 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 12 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 5 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 6 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 8 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 10 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 12 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 16 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 20 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 16 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 20 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.DIN 125A 14 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 14 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 18 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 22 ММ</t>
-  </si>
-  <si>
-    <t>ШАЙБА ОЦИНК.КУЗОВНАЯ DIN 9021 24 ММ</t>
-  </si>
-  <si>
-    <t>Номер лотка</t>
   </si>
 </sst>
 </file>
@@ -943,18 +943,18 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="52.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="52.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,16 +962,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>10138716</v>
       </c>
@@ -980,16 +980,16 @@
         <v>4606082001582</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>10138732</v>
       </c>
@@ -998,16 +998,16 @@
         <v>4606082001599</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>10138783</v>
       </c>
@@ -1016,16 +1016,16 @@
         <v>4606082001605</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>10138804</v>
       </c>
@@ -1034,16 +1034,16 @@
         <v>4606082001612</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>10138839</v>
       </c>
@@ -1052,16 +1052,16 @@
         <v>4606082001629</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10139145</v>
       </c>
@@ -1070,16 +1070,16 @@
         <v>4606082001711</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>10139161</v>
       </c>
@@ -1088,16 +1088,16 @@
         <v>4606082001728</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10139217</v>
       </c>
@@ -1106,16 +1106,16 @@
         <v>4606082001735</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>10139233</v>
       </c>
@@ -1124,16 +1124,16 @@
         <v>4606082001742</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10139284</v>
       </c>
@@ -1142,16 +1142,16 @@
         <v>4606082001759</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>13628067</v>
       </c>
@@ -1160,16 +1160,16 @@
         <v>4606082011031</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>13628075</v>
       </c>
@@ -1178,16 +1178,16 @@
         <v>4606082011048</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13628083</v>
       </c>
@@ -1196,16 +1196,16 @@
         <v>4606082011055</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13628091</v>
       </c>
@@ -1214,16 +1214,16 @@
         <v>4606082011062</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13978016</v>
       </c>
@@ -1232,16 +1232,16 @@
         <v>4606082016173</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13978091</v>
       </c>
@@ -1250,16 +1250,16 @@
         <v>4606082016142</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>13978198</v>
       </c>
@@ -1268,16 +1268,16 @@
         <v>4606082016159</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13978200</v>
       </c>
@@ -1286,16 +1286,16 @@
         <v>4606082039523</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>13978219</v>
       </c>
@@ -1304,16 +1304,16 @@
         <v>4606082016166</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>

</xml_diff>